<commit_message>
update excel, add index lighthouse result report
</commit_message>
<xml_diff>
--- a/docs/Optymalizacja_stron_kurs_dane.xlsx
+++ b/docs/Optymalizacja_stron_kurs_dane.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\frontend-optimisation-course\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E054969C-DC67-47B3-91A2-E32B979964B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2709F632-9DCA-4B8C-9CC3-035B881AF93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{3B773E87-3B6C-4DE5-919E-D150C5B524BC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{3B773E87-3B6C-4DE5-919E-D150C5B524BC}"/>
   </bookViews>
   <sheets>
     <sheet name="WebPageTest" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Optymalizacja strony</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Summary</t>
+  </si>
+  <si>
+    <t>TODO - opracować PB</t>
   </si>
 </sst>
 </file>
@@ -288,7 +291,77 @@
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -942,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AED66D-E3E2-4688-87F5-1B0E1FAD45EB}">
   <dimension ref="C3:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E01207A-9242-4CC4-AF90-BCDE49C7F563}">
-  <dimension ref="C3"/>
+  <dimension ref="C3:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1188,6 +1261,11 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1197,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D63C05B-D3AF-4235-84AF-0DFB29B97807}">
   <dimension ref="C2:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1443,10 +1521,10 @@
     <mergeCell ref="E5:G5"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D16">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>"NIE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>"TAK"</formula>
     </cfRule>
     <cfRule type="iconSet" priority="4">

</xml_diff>